<commit_message>
TCL01 Study 1-101 testcases
</commit_message>
<xml_diff>
--- a/InputFiles/TC08_Canine_Filter_Study-TCL01.xlsx
+++ b/InputFiles/TC08_Canine_Filter_Study-TCL01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podagatlapalll2\Desktop\Commons_Automation-Lakshmi_March\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356DFE14-5DAE-4B5F-AD6E-6ABD56DE869A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DB8A84-3447-4E0B-A241-8F3F0A445201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>WebExcel</t>
   </si>
@@ -57,16 +57,7 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t>TC08_Canine_Filter_Study-TCL01_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC08_Canine_Filter_Study-TCL01_WebData.xlsx</t>
-  </si>
-  <si>
     <t>StudyFilesTab</t>
-  </si>
-  <si>
-    <t>cartQuery</t>
   </si>
   <si>
     <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
@@ -75,7 +66,7 @@
 OPTIONAL MATCH (f:file)-[*]-&gt;(c)
 OPTIONAL MATCH (sf:file)--&gt;(s)
 WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
- WHERE s.clinical_study_designation IN ['TCL01']
+ WHERE s.clinical_study_designation IN ['TCL01'] and demo.breed in ['Beagle']
 RETURN  
     count(distinct p) AS Programs,
     count(distinct s) AS Studies,
@@ -85,9 +76,77 @@
     count(distinct sf) AS `Study Files`</t>
   </si>
   <si>
+    <t>TC08_Canine_Filter_Study-TCL01_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>TC08_Canine_Filter_Study-TCL01_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+ WHERE s.clinical_study_designation IN ['TCL01'] and demo.breed in ['Beagle']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+order by c.case_id asc 
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+  WHERE s.clinical_study_designation IN ['TCL01'] and demo.breed in ['Beagle']
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc 
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+ MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['TCL01'] and demo.breed in['Beagle']  
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN coalesce(f.file_name, '') AS `File Name`, 
+        coalesce(f.file_type, '') AS `File Type`, 
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `File Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`
+order by f.filename asc
+limit 100</t>
+  </si>
+  <si>
     <t xml:space="preserve">  MATCH (f:file)--&gt;(s:study)
 MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
- WHERE s.clinical_study_designation IN ['TCL01']
+ WHERE s.clinical_study_designation IN ['TCL01'] and demo.breed in ['Beagle']
 WITH DISTINCT f,  s, c, demo, diag
 WITH
         f, c, demo, diag, s,
@@ -108,78 +167,9 @@
   coalesce(f.file_description, '') AS `Description`,
   coalesce(f.file_format, '') AS  Format,
   CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- WHERE s.clinical_study_designation IN ['TCL01']
-OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
-WITH
-        f, parent, c, demo, diag, s, samp,
-        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-        toInteger(floor(log(f.file_size)/log(1024))) as i,
-        2 as precision
-WITH
-        f, parent, c, demo, diag, s, samp,
-        f.file_size /(1024^i) AS value, 
-        10^precision AS factor,
-        units[i] as unit
-WITH    
-        f, parent, c, demo, diag, s, samp, unit,
-        round(factor * value)/factor AS size
-RETURN 
-        coalesce(f.file_name, '') AS `File Name`,
-        coalesce(f.file_type, '') AS `File Type`,
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-        coalesce(samp.sample_id, '') AS `Sample ID`,
-        coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(demo.breed,'') AS Breed ,
-        coalesce(diag.disease_term,'') AS Diagnosis</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
- WHERE s.clinical_study_designation IN ['TCL01']
-WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed,
-        coalesce(diag.disease_term,'') AS Diagnosis, 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
- WHERE s.clinical_study_designation IN ['TCL01']
-MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
-RETURN  
-       coalesce(c.case_id, '') AS `Case ID`,
-       coalesce(s.clinical_study_designation, '') AS `Study Code`,
-       coalesce(s.clinical_study_type, '') AS  `Study Type`,
-       coalesce(demo.breed, '') AS Breed ,
-       coalesce(diag.disease_term, '') AS Diagnosis ,
-       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-       coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
-       coalesce(demo.sex, '') AS Sex,
-       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
-       coalesce(diag.best_response, '') AS `Response to Treatment`,
-       coalesce(co.cohort_description, '') AS `Cohort`</t>
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+order by f.filename asc
+limit 100</t>
   </si>
 </sst>
 </file>
@@ -549,21 +539,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" customWidth="1"/>
-    <col min="4" max="4" width="75.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="58.1796875" customWidth="1"/>
+    <col min="3" max="3" width="51.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" customWidth="1"/>
+    <col min="6" max="6" width="31.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -574,56 +566,47 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="390" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="315" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -631,36 +614,30 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>